<commit_message>
Scripts and new colors
</commit_message>
<xml_diff>
--- a/data/New Routes/Pop.xlsx
+++ b/data/New Routes/Pop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="22035" windowHeight="11310"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="22035" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Athens</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>TO</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>SPOP</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,6 +1139,9 @@
       <c r="H2" s="6">
         <v>54</v>
       </c>
+      <c r="I2" s="4">
+        <v>646.70000000000005</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1182,6 +1191,9 @@
       <c r="H4" s="6">
         <v>50</v>
       </c>
+      <c r="I4" s="4">
+        <v>65.12</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1205,6 +1217,9 @@
       <c r="H5" s="6">
         <v>55</v>
       </c>
+      <c r="I5" s="4">
+        <v>5263.5494509999999</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1228,6 +1243,9 @@
       <c r="H6" s="6">
         <v>8</v>
       </c>
+      <c r="I6" s="4">
+        <v>1187</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1277,6 +1295,9 @@
       <c r="H8" s="6">
         <v>31</v>
       </c>
+      <c r="I8" s="4">
+        <v>1240.7936</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1300,6 +1321,9 @@
       <c r="H9" s="6">
         <v>16</v>
       </c>
+      <c r="I9" s="4">
+        <v>334.9</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1323,6 +1347,9 @@
       <c r="H10" s="6">
         <v>5</v>
       </c>
+      <c r="I10" s="4">
+        <v>334.9</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1346,6 +1373,9 @@
       <c r="H11" s="6">
         <v>5</v>
       </c>
+      <c r="I11" s="4">
+        <v>1131.6761899999999</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1369,6 +1399,9 @@
       <c r="H12" s="6">
         <v>20</v>
       </c>
+      <c r="I12" s="4">
+        <v>950.22349710000003</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1392,6 +1425,9 @@
       <c r="H13" s="6">
         <v>25</v>
       </c>
+      <c r="I13" s="4">
+        <v>2395.6781559999999</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1415,6 +1451,9 @@
       <c r="H14" s="6">
         <v>38</v>
       </c>
+      <c r="I14" s="4">
+        <v>1917.6477950000001</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1462,7 +1501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1485,7 +1524,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1547,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1530,8 +1569,11 @@
       <c r="H19" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="4">
+        <v>60.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1553,8 +1595,11 @@
       <c r="H20" s="6">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="4">
+        <v>60.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1576,8 +1621,11 @@
       <c r="H21" s="6">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="4">
+        <v>290.85833330000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1599,8 +1647,11 @@
       <c r="H22" s="6">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="4">
+        <v>387.76777779999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1622,8 +1673,11 @@
       <c r="H23" s="6">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="4">
+        <v>190.36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1646,7 +1700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1669,7 +1723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1692,7 +1746,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1715,7 +1769,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1738,7 +1792,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1761,7 +1815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1783,8 +1837,11 @@
       <c r="H30" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I30" s="4">
+        <v>203.15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1806,8 +1863,11 @@
       <c r="H31" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I31" s="4">
+        <v>203.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1852,6 +1912,9 @@
       <c r="H33" s="6">
         <v>6</v>
       </c>
+      <c r="I33" s="4">
+        <v>698.4</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
@@ -1898,6 +1961,9 @@
       <c r="H35" s="6">
         <v>50</v>
       </c>
+      <c r="I35" s="4">
+        <v>581.57500000000005</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C36" s="5" t="s">
@@ -1949,6 +2015,9 @@
       <c r="H38" s="6">
         <v>51</v>
       </c>
+      <c r="I38" s="4">
+        <v>119.123</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C39" s="5" t="s">
@@ -2000,6 +2069,9 @@
       <c r="H41" s="6">
         <v>21</v>
       </c>
+      <c r="I41" s="4">
+        <v>634.04</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
@@ -2017,6 +2089,9 @@
       <c r="H42" s="6">
         <v>22</v>
       </c>
+      <c r="I42" s="4">
+        <v>1129</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
@@ -2035,7 +2110,7 @@
         <v>47</v>
       </c>
       <c r="I43" s="4">
-        <v>1669.7261900000001</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2128,8 +2203,11 @@
       <c r="H48" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="4">
+        <v>634.04</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="5" t="s">
         <v>57</v>
       </c>
@@ -2145,8 +2223,11 @@
       <c r="H49" s="6">
         <v>34</v>
       </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="4">
+        <v>197.41</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="5" t="s">
         <v>58</v>
       </c>
@@ -2162,8 +2243,11 @@
       <c r="H50" s="6">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="4">
+        <v>197.41</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="5" t="s">
         <v>26</v>
       </c>
@@ -2180,7 +2264,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="5" t="s">
         <v>27</v>
       </c>
@@ -2197,7 +2281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C53" s="5" t="s">
         <v>28</v>
       </c>
@@ -2214,7 +2298,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="5" t="s">
         <v>29</v>
       </c>
@@ -2231,7 +2315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="5" t="s">
         <v>30</v>
       </c>
@@ -2248,7 +2332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C56" s="5" t="s">
         <v>31</v>
       </c>
@@ -2265,7 +2349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C57" s="5" t="s">
         <v>32</v>
       </c>
@@ -2282,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C58" s="5" t="s">
         <v>33</v>
       </c>
@@ -2299,7 +2383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F59" s="6">
         <v>59</v>
       </c>
@@ -2310,7 +2394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F60" s="6">
         <v>60</v>
       </c>
@@ -2321,7 +2405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F61" s="6">
         <v>61</v>
       </c>
@@ -2332,7 +2416,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F62" s="6">
         <v>62</v>
       </c>
@@ -2343,7 +2427,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F63" s="6">
         <v>63</v>
       </c>
@@ -2354,7 +2438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F64" s="6">
         <v>64</v>
       </c>
@@ -2560,12 +2644,989 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>646.70000000000005</v>
+      </c>
+      <c r="C2">
+        <f>(B2-MIN($B$2:$B$81))/(MAX($B$2:$B$81)-MIN($B$2:$B$81))</f>
+        <v>0.1052582322004415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>243.8</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C66" si="0">(B3-MIN($B$2:$B$81))/(MAX($B$2:$B$81)-MIN($B$2:$B$81))</f>
+        <v>3.9681393243339476E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>65.12</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0599066152609788E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5263.5494509999999</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85670621665666358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1187</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.1931985799009186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1669.7261900000001</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.27176809497166926</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1240.7936</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.20195413771705847</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>334.9</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>5.4509018036072138E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>334.9</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>5.4509018036072138E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1131.6761899999999</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.18419396193402032</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>950.22349710000003</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.15466034560084638</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2395.6781559999999</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.38992554139751584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1917.6477950000001</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.3121203291862914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <v>60.25</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="0"/>
+        <v>9.8064148601772066E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <v>60.25</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="0"/>
+        <v>9.8064148601772066E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>290.85833330000003</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="0"/>
+        <v>4.7340705093435603E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <v>387.76777779999998</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="0"/>
+        <v>6.3113887112295652E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <v>190.36</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0983388095988933E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4">
+        <v>203.15</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3065115001576759E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4">
+        <v>203.15</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3065115001576759E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4">
+        <v>698.4</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="0"/>
+        <v>0.11367303134187155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4">
+        <v>581.57500000000005</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="0"/>
+        <v>9.4658352237469864E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>38</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>40</v>
+      </c>
+      <c r="B38" s="4">
+        <v>119.123</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="0"/>
+        <v>1.938870634670356E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>42</v>
+      </c>
+      <c r="B39" s="4">
+        <v>0</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>44</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>37</v>
+      </c>
+      <c r="B41" s="4">
+        <v>634.04</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10319766436426152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>39</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1129</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="0"/>
+        <v>0.18375837970356956</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1129</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="0"/>
+        <v>0.18375837970356956</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4">
+        <v>6143.9375</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4">
+        <v>6143.9375</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>46</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4">
+        <v>634.04</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10319766436426152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4">
+        <v>197.41</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2130860706183942E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4">
+        <v>197.41</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2130860706183942E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4">
+        <v>0</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>52</v>
+      </c>
+      <c r="B52" s="4">
+        <v>0</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>53</v>
+      </c>
+      <c r="B53" s="4">
+        <v>0</v>
+      </c>
+      <c r="C53" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>54</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0</v>
+      </c>
+      <c r="C54" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+      <c r="C55" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>56</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4">
+        <v>0</v>
+      </c>
+      <c r="C57" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0</v>
+      </c>
+      <c r="C58" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4">
+        <v>0</v>
+      </c>
+      <c r="C59" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4">
+        <v>0</v>
+      </c>
+      <c r="C60" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>61</v>
+      </c>
+      <c r="B61" s="4">
+        <v>0</v>
+      </c>
+      <c r="C61" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4">
+        <v>0</v>
+      </c>
+      <c r="C62" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4">
+        <v>0</v>
+      </c>
+      <c r="C63" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4">
+        <v>0</v>
+      </c>
+      <c r="C64" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>65</v>
+      </c>
+      <c r="B65" s="4">
+        <v>0</v>
+      </c>
+      <c r="C65" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0</v>
+      </c>
+      <c r="C66" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>67</v>
+      </c>
+      <c r="B67" s="4">
+        <v>0</v>
+      </c>
+      <c r="C67" s="6">
+        <f t="shared" ref="C67:C81" si="1">(B67-MIN($B$2:$B$81))/(MAX($B$2:$B$81)-MIN($B$2:$B$81))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>68</v>
+      </c>
+      <c r="B68" s="4">
+        <v>0</v>
+      </c>
+      <c r="C68" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>69</v>
+      </c>
+      <c r="B69" s="4">
+        <v>0</v>
+      </c>
+      <c r="C69" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>70</v>
+      </c>
+      <c r="B70" s="4">
+        <v>0</v>
+      </c>
+      <c r="C70" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>8</v>
+      </c>
+      <c r="B71" s="4">
+        <v>0</v>
+      </c>
+      <c r="C71" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>71</v>
+      </c>
+      <c r="B72" s="4">
+        <v>0</v>
+      </c>
+      <c r="C72" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>72</v>
+      </c>
+      <c r="B73" s="4">
+        <v>0</v>
+      </c>
+      <c r="C73" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>73</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0</v>
+      </c>
+      <c r="C74" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>74</v>
+      </c>
+      <c r="B75" s="4">
+        <v>0</v>
+      </c>
+      <c r="C75" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>75</v>
+      </c>
+      <c r="B76" s="4">
+        <v>0</v>
+      </c>
+      <c r="C76" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4">
+        <v>0</v>
+      </c>
+      <c r="C77" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>77</v>
+      </c>
+      <c r="B78" s="4">
+        <v>0</v>
+      </c>
+      <c r="C78" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>78</v>
+      </c>
+      <c r="B79" s="4">
+        <v>0</v>
+      </c>
+      <c r="C79" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>79</v>
+      </c>
+      <c r="B80" s="4">
+        <v>0</v>
+      </c>
+      <c r="C80" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>80</v>
+      </c>
+      <c r="B81" s="4">
+        <v>0</v>
+      </c>
+      <c r="C81" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>